<commit_message>
Add sample files for testing backend
</commit_message>
<xml_diff>
--- a/documentation/DbModelDraft.xlsx
+++ b/documentation/DbModelDraft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BITSProject\CPADAssignment-1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E047C622-B9E9-41D3-A0CC-2CBF05405492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E682AD36-298F-4F7B-BA68-9068C505B1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7569AB63-CD0F-407D-A1C1-8FB414BFCF75}"/>
   </bookViews>
@@ -514,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1071B826-3578-430E-AA51-BEF23384EF74}">
   <dimension ref="C3:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17:E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>